<commit_message>
generating the nominal part of the report for bibliography products
</commit_message>
<xml_diff>
--- a/data/producao-tecnica.xlsx
+++ b/data/producao-tecnica.xlsx
@@ -171,7 +171,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Quais são as produções do tipo Produção técnica, publicadas entre 2022 e 2025,  cujos nomes dos autores são Alessandro Botelho Bovo, Alireza Mohebi Ashtiani, Bruno Samways dos Santos, Danilo Sipoli Sanches, Edson Luiz Valmorbida, Elizabeth Mie Hashimoto, Henrique Yoshikazu Shishido, Jose Luis Dalto, José Ângelo Ferreira, Marco Antonio Ferreira, Marcos Jeronimo Goroski Rambalducci, Pedro Rochavetz de Lara Andrade, Rafael Henrique Palma Lima ou Willian Massami Watanabe?</t>
+          <t>Quais são as produções do tipo Produção técnica, publicadas entre 2022 e 2025,  cujos nomes dos autores são Alessandro Botelho Bovo, Alireza Mohebi Ashtiani, Bruno Samways dos Santos, Danilo Sipoli Sanches, Edson Luiz Valmorbida, Elizabeth Mie Hashimoto, Henrique Yoshikazu Shishido, Jose Luis Dalto, José Ângelo Ferreira, Marco Antonio Ferreira, Marcos Jeronimo Goroski Rambalducci, Pedro Rochavetz de Lara Andrade, Rafael Henrique Palma Lima, Reginaldo Fidelis, Rogerio Tondato ou Willian Massami Watanabe?</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -203,7 +203,7 @@
     <row r="2" customHeight="true" ht="35.0">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Arquivo gerado em 18/12/2025 às 15:11:04 pela Plataforma Stela Experta. 
+          <t>Arquivo gerado em 18/12/2025 às 18:46:58 pela Plataforma Stela Experta. 
 Última atualização dos CV-Lattes no Experta: 12/12/2025</t>
         </is>
       </c>

</xml_diff>